<commit_message>
update formatting in spreadsheet
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payamazadi/code/pasureaudit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD788ED-069C-4349-9AC2-B1B0EFCDC29A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7104F195-4A4A-C641-8EC9-A724179BD404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{B4068717-85FA-DA46-B2DB-E29CD6EF2930}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -108,10 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,6 +238,112 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1DB8-3942-BAE8-A1447803A9AD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-1DB8-3942-BAE8-A1447803A9AD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1DB8-3942-BAE8-A1447803A9AD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$1:$C$1</c:f>
@@ -255,7 +362,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$C$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>5454173</c:v>
@@ -358,7 +465,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -550,6 +657,83 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0C1C-8D47-9A9E-6F54B20E8B44}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$1:$C$1</c:f>
@@ -568,7 +752,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1463410</c:v>
@@ -670,7 +854,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2217,7 +2401,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2240,11 +2424,11 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>B21</f>
         <v>5454173</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>B26</f>
         <v>5455192</v>
       </c>
@@ -2257,15 +2441,15 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f>B20</f>
         <v>1463410</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>B25</f>
         <v>1324826</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <f>B3-C3</f>
         <v>138584</v>
       </c>
@@ -2274,15 +2458,15 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f>B2+B3</f>
         <v>6917583</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>C2+C3</f>
         <v>6780018</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <f>B4-C4</f>
         <v>137565</v>
       </c>
@@ -2296,7 +2480,7 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>6917583</v>
       </c>
     </row>
@@ -2304,7 +2488,7 @@
       <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>1463410</v>
       </c>
     </row>
@@ -2312,21 +2496,25 @@
       <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <f>B19-B20</f>
         <v>5454173</v>
       </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>6780018</v>
       </c>
     </row>
@@ -2334,7 +2522,7 @@
       <c r="A25" t="s">
         <v>7</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>1324826</v>
       </c>
     </row>
@@ -2342,7 +2530,7 @@
       <c r="A26" t="s">
         <v>6</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <f>B24-B25</f>
         <v>5455192</v>
       </c>

</xml_diff>

<commit_message>
fix bug in refactor, update filepath, update comparison (new data released)
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payamazadi/code/pasureaudit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7104F195-4A4A-C641-8EC9-A724179BD404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF8F1EE-840D-CB43-A258-E94EB43574C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{B4068717-85FA-DA46-B2DB-E29CD6EF2930}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>NYT</t>
   </si>
@@ -42,33 +42,41 @@
     <t>SURE Dump</t>
   </si>
   <si>
-    <t>Counties except Allegheny &amp; Philly</t>
-  </si>
-  <si>
-    <t>Allegheny and Philly</t>
-  </si>
-  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Allegheny &amp; Philly only</t>
   </si>
   <si>
     <t>Remaining counties</t>
   </si>
   <si>
-    <t>Allegheny &amp; Philly Only</t>
+    <t>Difference</t>
   </si>
   <si>
-    <t>Difference</t>
+    <t>Counties except Allegheny</t>
+  </si>
+  <si>
+    <t>Allegheny</t>
+  </si>
+  <si>
+    <t>Allegheny only</t>
+  </si>
+  <si>
+    <t>Allegheny - Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,11 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,7 +183,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>counties except Allegheny &amp; Philly</a:t>
+              <a:t>counties except Allegheny</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -223,7 +233,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Counties except Allegheny &amp; Philly</c:v>
+                  <c:v>Counties except Allegheny</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -365,10 +375,10 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5454173</c:v>
+                  <c:v>6195550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5455192</c:v>
+                  <c:v>6200003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,7 +599,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>2020 Pres Votes vs Ballots Tallied only Allegheny &amp; Philly</a:t>
+              <a:t>2020 Pres Votes vs Ballots Tallied only Allegheny</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
@@ -642,7 +652,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Allegheny and Philly</c:v>
+                  <c:v>Allegheny</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -755,10 +765,10 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1463410</c:v>
+                  <c:v>722033</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1324826</c:v>
+                  <c:v>607358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2030,14 +2040,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2066,14 +2076,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2398,18 +2408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4898D22-CC9C-7548-8ACA-389C20DEF350}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2417,46 +2429,54 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <f>B21</f>
-        <v>5454173</v>
+        <v>6195550</v>
       </c>
       <c r="C2" s="1">
         <f>B26</f>
-        <v>5455192</v>
-      </c>
-      <c r="D2" s="2">
+        <v>6200003</v>
+      </c>
+      <c r="D2" s="3">
         <f>B2-C2</f>
-        <v>-1019</v>
-      </c>
+        <v>-4453</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <f>B20</f>
-        <v>1463410</v>
+        <v>722033</v>
       </c>
       <c r="C3" s="1">
         <f>B25</f>
-        <v>1324826</v>
-      </c>
-      <c r="D3" s="3">
+        <v>607358</v>
+      </c>
+      <c r="D3" s="2">
         <f>B3-C3</f>
-        <v>138584</v>
-      </c>
+        <v>114675</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <f>B2+B3</f>
@@ -2464,76 +2484,98 @@
       </c>
       <c r="C4" s="1">
         <f>C2+C3</f>
-        <v>6780018</v>
-      </c>
-      <c r="D4" s="3">
+        <v>6807361</v>
+      </c>
+      <c r="D4" s="2">
         <f>B4-C4</f>
-        <v>137565</v>
-      </c>
+        <v>110222</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <f>D3-D4</f>
+        <v>4453</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>6917583</v>
       </c>
+      <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1">
-        <v>1463410</v>
-      </c>
+        <v>722033</v>
+      </c>
+      <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1">
         <f>B19-B20</f>
-        <v>5454173</v>
-      </c>
+        <v>6195550</v>
+      </c>
+      <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>6780018</v>
-      </c>
+        <v>6807361</v>
+      </c>
+      <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1">
-        <v>1324826</v>
-      </c>
+        <v>607358</v>
+      </c>
+      <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B26" s="1">
         <f>B24-B25</f>
-        <v>5455192</v>
-      </c>
+        <v>6200003</v>
+      </c>
+      <c r="I26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update comparison spreadsheet for new data
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payamazadi/code/pasureaudit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF8F1EE-840D-CB43-A258-E94EB43574C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1510E53-E539-274A-B87E-1D0F7D49AD5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{B4068717-85FA-DA46-B2DB-E29CD6EF2930}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>NYT</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Allegheny only</t>
-  </si>
-  <si>
-    <t>Allegheny - Total</t>
   </si>
 </sst>
 </file>
@@ -116,13 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2411,7 +2409,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2495,13 +2493,7 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3">
-        <f>D3-D4</f>
-        <v>4453</v>
-      </c>
+      <c r="D5" s="6"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>

</xml_diff>